<commit_message>
master: updated risk plan
</commit_message>
<xml_diff>
--- a/docs/project_management/risk_management/risk_management.xlsx
+++ b/docs/project_management/risk_management/risk_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070497\OneDrive - SAP SE\Workspaces\IdeaProjects\dashup\docs\project_management\risk_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{F900A722-4BC7-434F-A779-E93B6799B648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{81AAE4F9-6E70-4E16-B7E1-35A99082919F}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{F900A722-4BC7-434F-A779-E93B6799B648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2B5ED2B8-D12F-495C-98EF-3354FBFCF2E9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F5417B3B-7B9C-4EF2-920C-2857935D6879}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{F5417B3B-7B9C-4EF2-920C-2857935D6879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Risk name</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Native browser support or changes in specifications of web platform APIs</t>
+  </si>
+  <si>
+    <t>Hardware problems</t>
+  </si>
+  <si>
+    <t>Laptop crashes multiple times while working, impacting workflow severely</t>
+  </si>
+  <si>
+    <t>Contacting IT Support as soon as possible</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -227,6 +236,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -236,14 +263,7 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -255,7 +275,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -277,19 +304,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{212E89E3-D5FB-4B0D-92D1-B0CCC035979A}" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Heading 3" dataCellStyle="Heading 3">
-  <autoFilter ref="A1:G11" xr:uid="{F5CC6EB2-9EF3-41B5-BABE-F8529B403134}"/>
-  <sortState ref="A2:G11">
-    <sortCondition descending="1" ref="G1:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{212E89E3-D5FB-4B0D-92D1-B0CCC035979A}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Heading 3" dataCellStyle="Heading 3">
+  <autoFilter ref="A1:G12" xr:uid="{F5CC6EB2-9EF3-41B5-BABE-F8529B403134}"/>
+  <sortState ref="A2:G12">
+    <sortCondition descending="1" ref="G1:G12"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8C3EC4D7-9E32-45FF-BE37-5AE0B7813C4A}" name="Risk name" dataDxfId="2" dataCellStyle="Heading 3"/>
-    <tableColumn id="2" xr3:uid="{14DCD268-BCE7-4F8C-8A43-9C82B7C73950}" name="Risk description" dataDxfId="0" dataCellStyle="Heading 3"/>
-    <tableColumn id="3" xr3:uid="{8138ACB1-79F6-479E-B4C0-C12F2A0184CF}" name="Risk probality of occurance" dataDxfId="1" dataCellStyle="Heading 3"/>
-    <tableColumn id="4" xr3:uid="{2B602890-C088-4815-B9B2-18528650C3C1}" name="Risk impact / damage" dataDxfId="5" dataCellStyle="Heading 3"/>
-    <tableColumn id="6" xr3:uid="{EC8E0F99-6C9D-4163-B459-F10E7BB39764}" name="Risk mitigation" dataDxfId="3" dataCellStyle="Heading 3"/>
-    <tableColumn id="7" xr3:uid="{EFCB6C56-5588-49FF-AF1A-5DDB601F6AE6}" name="Person in charge" dataDxfId="4" dataCellStyle="Heading 3"/>
-    <tableColumn id="8" xr3:uid="{9DA67F14-8F0E-4C22-9ACE-0DDB972C6703}" name="Risk facor" dataDxfId="6" dataCellStyle="Heading 3">
+    <tableColumn id="1" xr3:uid="{8C3EC4D7-9E32-45FF-BE37-5AE0B7813C4A}" name="Risk name" dataDxfId="6" dataCellStyle="Heading 3"/>
+    <tableColumn id="2" xr3:uid="{14DCD268-BCE7-4F8C-8A43-9C82B7C73950}" name="Risk description" dataDxfId="5" dataCellStyle="Heading 3"/>
+    <tableColumn id="3" xr3:uid="{8138ACB1-79F6-479E-B4C0-C12F2A0184CF}" name="Risk probality of occurance" dataDxfId="4" dataCellStyle="Heading 3"/>
+    <tableColumn id="4" xr3:uid="{2B602890-C088-4815-B9B2-18528650C3C1}" name="Risk impact / damage" dataDxfId="3" dataCellStyle="Heading 3"/>
+    <tableColumn id="6" xr3:uid="{EC8E0F99-6C9D-4163-B459-F10E7BB39764}" name="Risk mitigation" dataDxfId="2" dataCellStyle="Heading 3"/>
+    <tableColumn id="7" xr3:uid="{EFCB6C56-5588-49FF-AF1A-5DDB601F6AE6}" name="Person in charge" dataDxfId="1" dataCellStyle="Heading 3"/>
+    <tableColumn id="8" xr3:uid="{9DA67F14-8F0E-4C22-9ACE-0DDB972C6703}" name="Risk facor" dataDxfId="0" dataCellStyle="Heading 3">
       <calculatedColumnFormula>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -594,23 +621,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D748AAB-DC3E-4DAC-BECD-004010136645}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="2" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="23" style="2" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -633,199 +662,199 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="6">
         <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="6">
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="11">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="11">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+      <c r="G6" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="D4" s="6">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C9" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="6">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="D6" s="6">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="G9" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
         <v>0.5</v>
       </c>
-      <c r="D7" s="6">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="6">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="6">
-        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -833,7 +862,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D10" s="6">
         <v>4</v>
@@ -846,29 +875,53 @@
       </c>
       <c r="G10" s="6">
         <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D11" s="6">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="6">
+        <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="10">
         <v>0.01</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="12">
         <v>10</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="12">
         <f>Table1[Risk probality of occurance]*Table1[Risk impact / damage]</f>
         <v>0.1</v>
       </c>

</xml_diff>

<commit_message>
master: updated some other documents
</commit_message>
<xml_diff>
--- a/docs/project_management/risk_management/risk_management.xlsx
+++ b/docs/project_management/risk_management/risk_management.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070497\OneDrive - SAP SE\Workspaces\IdeaProjects\dashup\docs\project_management\risk_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{F900A722-4BC7-434F-A779-E93B6799B648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2B5ED2B8-D12F-495C-98EF-3354FBFCF2E9}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{F900A722-4BC7-434F-A779-E93B6799B648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{29510756-05F2-4420-86B1-4C5D105A79A3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{F5417B3B-7B9C-4EF2-920C-2857935D6879}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" activeTab="2" xr2:uid="{F5417B3B-7B9C-4EF2-920C-2857935D6879}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart2" sheetId="3" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -301,6 +303,1612 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="928802728"/>
+        <c:axId val="928807976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="928802728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="928807976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="928807976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="928802728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="630200408"/>
+        <c:axId val="630200736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="630200408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="630200736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="630200736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="630200408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{32A2ED97-93DE-4985-A717-04779AA98E5A}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A0055BA2-CF8C-453E-AC3D-0BA36855F06B}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAFAA9D8-AC78-43D5-A09D-F486C00BCB5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1737EB97-A45C-4CA7-911D-B65A1CB12EB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D748AAB-DC3E-4DAC-BECD-004010136645}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>